<commit_message>
Added "Alternative ID" attribute
</commit_message>
<xml_diff>
--- a/epic/latest/segmentation-mask-object-by-feature.xlsx
+++ b/epic/latest/segmentation-mask-object-by-feature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josefhardi/Documents/Code/dataset-metadata-spreadsheet/epic/latest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9D7FCD-D947-2B4C-9417-1DCE8BFBE8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3DC701-355F-8043-96F6-C607048FBEC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="400" yWindow="1460" windowWidth="34160" windowHeight="19960" xr2:uid="{C4595F7F-ACBB-FB4D-A7BB-AF16387AE2E4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>Type</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Object ID</t>
+  </si>
+  <si>
+    <t>Alternative ID</t>
   </si>
 </sst>
 </file>
@@ -636,11 +639,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5681F060-6354-5B42-B552-D4F093A27A7D}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F17" sqref="F17"/>
+      <selection pane="topRight" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -788,113 +791,117 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="54" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="54" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" s="11" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" s="11" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J10" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
+      <c r="E11" s="12"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
@@ -950,26 +957,36 @@
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="10"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="10"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="10"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="10"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="10"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="10"/>
     </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="10"/>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="aTBKL0w1f51eMVQSJ+tZk3q/36gwQlYXY4mXjMAfxQLl6Kw7pVDkADGBdzBDjM+LpgZGYQyHF1sEIlCeruPdxA==" saltValue="TmZKBWIdKTKjhq14QsW5nQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="kQvYcocs//yQTWIiIZG3o746ASdnQ0jvTEX4bNGhWfTzXR6IqtNorzjjTGDf+P/v/0Ascz9O9hyw/Nxbzik0ug==" saltValue="7CjbiBT6uyeFFwFNeM106g==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Metadata schema ID row
</commit_message>
<xml_diff>
--- a/epic/latest/segmentation-mask-object-by-feature.xlsx
+++ b/epic/latest/segmentation-mask-object-by-feature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josefhardi/Documents/Code/dataset-metadata-spreadsheet/epic/latest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3DC701-355F-8043-96F6-C607048FBEC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D387569-FB24-1E44-986F-5796B2693D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="400" yWindow="1460" windowWidth="34160" windowHeight="19960" xr2:uid="{C4595F7F-ACBB-FB4D-A7BB-AF16387AE2E4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
   <si>
     <t>Type</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>Alternative ID</t>
+  </si>
+  <si>
+    <t>Header schema ID</t>
+  </si>
+  <si>
+    <t>831aa83b-d217-4906-9a7f-46e859cfc945</t>
   </si>
 </sst>
 </file>
@@ -261,29 +267,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
@@ -303,6 +288,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -639,354 +654,370 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5681F060-6354-5B42-B552-D4F093A27A7D}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K7" sqref="K7"/>
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" style="9" customWidth="1"/>
-    <col min="2" max="10" width="31.6640625" style="9" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="8"/>
+    <col min="1" max="1" width="28.83203125" style="2" customWidth="1"/>
+    <col min="2" max="10" width="31.6640625" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J2" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J3" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J4" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="288" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:10" ht="288" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J5" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J6" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" ht="54" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:10" ht="54" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J9" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:10" s="11" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B11" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C11" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D11" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E11" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F11" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G11" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H11" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I11" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J11" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
+    <row r="12" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B18" s="10"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="10"/>
+      <c r="B19" s="3"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" s="10"/>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21" s="10"/>
+      <c r="B21" s="3"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22" s="10"/>
+      <c r="B22" s="3"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B23" s="10"/>
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="kQvYcocs//yQTWIiIZG3o746ASdnQ0jvTEX4bNGhWfTzXR6IqtNorzjjTGDf+P/v/0Ascz9O9hyw/Nxbzik0ug==" saltValue="7CjbiBT6uyeFFwFNeM106g==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="5ytuhyRfSuDQRZ5irLidhrROqLzQmyeufUY+IqGaBq1xyQRksin6GLnZjHXIFrm2fTRH7pkYuSitvRjDUpyN1A==" saltValue="ohSx21rI30+cjnh8QWmQDA==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removing "Metadata schema ID" field
</commit_message>
<xml_diff>
--- a/epic/latest/segmentation-mask-object-by-feature.xlsx
+++ b/epic/latest/segmentation-mask-object-by-feature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josefhardi/Documents/Code/dataset-metadata-spreadsheet/epic/latest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D387569-FB24-1E44-986F-5796B2693D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661960C2-496C-1A4A-932A-C49D6CD0290B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="400" yWindow="1460" windowWidth="34160" windowHeight="19960" xr2:uid="{C4595F7F-ACBB-FB4D-A7BB-AF16387AE2E4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>Type</t>
   </si>
@@ -156,12 +156,6 @@
   </si>
   <si>
     <t>Alternative ID</t>
-  </si>
-  <si>
-    <t>Header schema ID</t>
-  </si>
-  <si>
-    <t>831aa83b-d217-4906-9a7f-46e859cfc945</t>
   </si>
 </sst>
 </file>
@@ -267,7 +261,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
@@ -289,34 +283,25 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -654,11 +639,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5681F060-6354-5B42-B552-D4F093A27A7D}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L4" sqref="L4"/>
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -670,269 +655,263 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
+        <v>7</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>10</v>
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J3" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="288" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+    <row r="4" spans="1:10" ht="288" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J4" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+    <row r="5" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J5" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-    </row>
-    <row r="8" spans="1:10" ht="54" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" ht="54" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-    </row>
-    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J8" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="12"/>
-    </row>
-    <row r="11" spans="1:10" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D10" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F10" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G10" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H10" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="I10" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="J10" s="12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="5"/>
+      <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -990,13 +969,6 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
@@ -1013,11 +985,8 @@
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="3"/>
-    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="5ytuhyRfSuDQRZ5irLidhrROqLzQmyeufUY+IqGaBq1xyQRksin6GLnZjHXIFrm2fTRH7pkYuSitvRjDUpyN1A==" saltValue="ohSx21rI30+cjnh8QWmQDA==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="9ZoDxdVNFuqjQR4xEqWJ8Cp1ZYBbk/2ohSn046oVrgL+w8qd7P+7FSTGRqsiT3+FyujkK3IJuUEd4RTTF0J1BQ==" saltValue="CFsTAuGO85RtlxjqtNESiQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>